<commit_message>
Backup QR Scanner data - 2025-08-23T05:07:09.223Z - Cache Bust: 1755925629223
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2728_Anatomy_checklist1755925035146_5edfa2692bdacc5e6ee805c626c50cb44cebb065f092d9a1067d89f74dacd326.xlsx
+++ b/log_history/Y5_B2728_Anatomy_checklist1755925035146_5edfa2692bdacc5e6ee805c626c50cb44cebb065f092d9a1067d89f74dacd326.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -442,29 +442,9 @@
         <v>admin@admin.com</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>654321</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Anatomy</v>
-      </c>
-      <c r="C3" t="str">
-        <v>23/08/2025</v>
-      </c>
-      <c r="D3" t="str">
-        <v>07:57:20</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F3" t="str">
-        <v>admin@admin.com</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>